<commit_message>
Added Environment as OppossiteProcessorType
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/v2/15_graph_solver_example.xlsx
+++ b/backend_tests/z_input_files/v2/15_graph_solver_example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="178">
   <si>
     <t xml:space="preserve">Parameter</t>
   </si>
@@ -753,8 +753,8 @@
   </sheetPr>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="H38:H39 A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -856,7 +856,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="1" sqref="H38:H39 C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1033,7 +1033,7 @@
   <dimension ref="A1:AMJ26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="H38:H39 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1604,7 +1604,7 @@
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="H38:H39 B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2261,8 +2261,8 @@
   </sheetPr>
   <dimension ref="A1:V40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D28" activeCellId="1" sqref="H38:H39 D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2860,7 +2860,7 @@
   <dimension ref="A1:V65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="1" sqref="H38:H39 H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2870,9 +2870,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="8.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="6.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="11.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="6.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="10.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="6.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="13.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="5.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="5.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="4" width="5.55"/>
@@ -2966,6 +2966,9 @@
       <c r="G2" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="H2" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="L2" s="4" t="n">
         <v>0.1285149</v>
       </c>
@@ -2986,6 +2989,9 @@
       <c r="G3" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="H3" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="L3" s="4" t="n">
         <v>0.1164551</v>
       </c>
@@ -3006,6 +3012,9 @@
       <c r="G4" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="H4" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="L4" s="4" t="n">
         <v>0.0810668396092578</v>
       </c>
@@ -3026,6 +3035,9 @@
       <c r="G5" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="H5" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="L5" s="4" t="n">
         <v>0.0810241451952682</v>
       </c>
@@ -3046,6 +3058,9 @@
       <c r="G6" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="H6" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="L6" s="4" t="n">
         <v>0.0125177909103313</v>
       </c>
@@ -3066,6 +3081,9 @@
       <c r="G7" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="H7" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="L7" s="4" t="n">
         <v>0.0125698253799858</v>
       </c>
@@ -3086,6 +3104,9 @@
       <c r="G8" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="H8" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="L8" s="4" t="n">
         <v>0.290807572629191</v>
       </c>
@@ -3106,6 +3127,9 @@
       <c r="G9" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="H9" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="L9" s="4" t="n">
         <v>0.284819139846198</v>
       </c>
@@ -3126,6 +3150,9 @@
       <c r="G10" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="H10" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="L10" s="4" t="n">
         <v>510.783090193891</v>
       </c>
@@ -3146,6 +3173,9 @@
       <c r="G11" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="H11" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="L11" s="4" t="n">
         <v>510.783090193891</v>
       </c>
@@ -3166,6 +3196,9 @@
       <c r="G12" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="H12" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="L12" s="4" t="n">
         <v>344.554124680908</v>
       </c>
@@ -3186,6 +3219,9 @@
       <c r="G13" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="H13" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="L13" s="4" t="n">
         <v>344.554124680908</v>
       </c>
@@ -3206,6 +3242,9 @@
       <c r="G14" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="H14" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="L14" s="4" t="n">
         <v>54.7726040228444</v>
       </c>
@@ -3226,6 +3265,9 @@
       <c r="G15" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="H15" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="L15" s="4" t="n">
         <v>54.7726040228444</v>
       </c>
@@ -3246,6 +3288,9 @@
       <c r="G16" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="H16" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="L16" s="4" t="n">
         <v>876.195771627155</v>
       </c>
@@ -3266,6 +3311,9 @@
       <c r="G17" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="H17" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="L17" s="4" t="n">
         <v>876.195771627155</v>
       </c>
@@ -3286,6 +3334,9 @@
       <c r="G18" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="H18" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="R18" s="4" t="s">
         <v>38</v>
       </c>
@@ -3303,6 +3354,9 @@
       <c r="G19" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="H19" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="R19" s="4" t="s">
         <v>38</v>
       </c>
@@ -3320,6 +3374,9 @@
       <c r="G20" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="H20" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="L20" s="4" t="n">
         <v>16.2712344327208</v>
       </c>
@@ -3340,6 +3397,9 @@
       <c r="G21" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="H21" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="L21" s="4" t="n">
         <v>16.2712344327208</v>
       </c>
@@ -3360,6 +3420,9 @@
       <c r="G22" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="H22" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="L22" s="4" t="n">
         <v>0.219509168287431</v>
       </c>
@@ -3380,6 +3443,9 @@
       <c r="G23" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="H23" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="L23" s="4" t="n">
         <v>0.219509168287431</v>
       </c>
@@ -3400,6 +3466,9 @@
       <c r="G24" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="H24" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="R24" s="4" t="s">
         <v>34</v>
       </c>
@@ -3416,6 +3485,9 @@
       </c>
       <c r="G25" s="4" t="s">
         <v>132</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="R25" s="4" t="s">
         <v>34</v>
@@ -4242,8 +4314,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H38" activeCellId="0" sqref="H38:H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4351,6 +4423,9 @@
       <c r="G2" s="0" t="s">
         <v>132</v>
       </c>
+      <c r="H2" s="0" t="s">
+        <v>49</v>
+      </c>
       <c r="L2" s="0" t="n">
         <v>14.639493</v>
       </c>
@@ -4372,6 +4447,9 @@
       <c r="G3" s="0" t="s">
         <v>133</v>
       </c>
+      <c r="H3" s="0" t="s">
+        <v>49</v>
+      </c>
       <c r="L3" s="0" t="n">
         <v>7.7147</v>
       </c>
@@ -4473,6 +4551,9 @@
       <c r="G8" s="0" t="s">
         <v>132</v>
       </c>
+      <c r="H8" s="0" t="s">
+        <v>49</v>
+      </c>
       <c r="L8" s="0" t="n">
         <v>0.423619</v>
       </c>
@@ -4493,6 +4574,9 @@
       <c r="G9" s="0" t="s">
         <v>133</v>
       </c>
+      <c r="H9" s="0" t="s">
+        <v>49</v>
+      </c>
       <c r="L9" s="0" t="n">
         <v>0.198178</v>
       </c>
@@ -4594,6 +4678,9 @@
       <c r="G14" s="0" t="s">
         <v>132</v>
       </c>
+      <c r="H14" s="0" t="s">
+        <v>49</v>
+      </c>
       <c r="L14" s="0" t="n">
         <v>0.483017507961291</v>
       </c>
@@ -4614,6 +4701,9 @@
       <c r="G15" s="0" t="s">
         <v>133</v>
       </c>
+      <c r="H15" s="0" t="s">
+        <v>49</v>
+      </c>
       <c r="L15" s="0" t="n">
         <v>0.318721995608352</v>
       </c>
@@ -4715,6 +4805,9 @@
       <c r="G20" s="0" t="s">
         <v>132</v>
       </c>
+      <c r="H20" s="0" t="s">
+        <v>49</v>
+      </c>
       <c r="L20" s="0" t="n">
         <v>31.1</v>
       </c>
@@ -4735,6 +4828,9 @@
       <c r="G21" s="0" t="s">
         <v>133</v>
       </c>
+      <c r="H21" s="0" t="s">
+        <v>49</v>
+      </c>
       <c r="L21" s="0" t="n">
         <v>21.2</v>
       </c>
@@ -4836,6 +4932,9 @@
       <c r="G26" s="0" t="s">
         <v>132</v>
       </c>
+      <c r="H26" s="0" t="s">
+        <v>49</v>
+      </c>
       <c r="L26" s="0" t="n">
         <v>11.000603</v>
       </c>
@@ -4856,6 +4955,9 @@
       <c r="G27" s="0" t="s">
         <v>133</v>
       </c>
+      <c r="H27" s="0" t="s">
+        <v>49</v>
+      </c>
       <c r="L27" s="0" t="n">
         <v>1.1</v>
       </c>
@@ -4957,6 +5059,9 @@
       <c r="G32" s="0" t="s">
         <v>132</v>
       </c>
+      <c r="H32" s="0" t="s">
+        <v>49</v>
+      </c>
       <c r="L32" s="0" t="n">
         <v>4.388</v>
       </c>
@@ -4977,6 +5082,9 @@
       <c r="G33" s="0" t="s">
         <v>133</v>
       </c>
+      <c r="H33" s="0" t="s">
+        <v>49</v>
+      </c>
       <c r="L33" s="0" t="n">
         <v>4.34</v>
       </c>
@@ -5078,6 +5186,9 @@
       <c r="G38" s="0" t="s">
         <v>132</v>
       </c>
+      <c r="H38" s="0" t="s">
+        <v>49</v>
+      </c>
       <c r="L38" s="0" t="n">
         <v>8.69</v>
       </c>
@@ -5097,6 +5208,9 @@
       </c>
       <c r="G39" s="0" t="s">
         <v>133</v>
+      </c>
+      <c r="H39" s="0" t="s">
+        <v>49</v>
       </c>
       <c r="L39" s="0" t="n">
         <v>2.79</v>
@@ -5207,7 +5321,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="1" sqref="H38:H39 D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5650,7 +5764,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
+      <selection pane="topLeft" activeCell="G26" activeCellId="1" sqref="H38:H39 G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Fixed excel: removed conflicting crop->processing scale
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/v2/15_graph_solver_example.xlsx
+++ b/backend_tests/z_input_files/v2/15_graph_solver_example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="178">
   <si>
     <t xml:space="preserve">Parameter</t>
   </si>
@@ -754,7 +754,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="H38:H39 A6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -856,7 +856,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="1" sqref="H38:H39 C13"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1033,7 +1033,7 @@
   <dimension ref="A1:AMJ26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="H38:H39 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1604,7 +1604,7 @@
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="H38:H39 B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2262,7 +2262,7 @@
   <dimension ref="A1:V40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="1" sqref="H38:H39 D28"/>
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2860,7 +2860,7 @@
   <dimension ref="A1:V65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="1" sqref="H38:H39 H2"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2870,7 +2870,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="8.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="6.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="6.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="6.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="10.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="13.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="5.96"/>
@@ -4314,8 +4314,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H38" activeCellId="0" sqref="H38:H39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H38" activeCellId="0" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5321,7 +5321,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="1" sqref="H38:H39 D17"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5761,10 +5761,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G26" activeCellId="1" sqref="H38:H39 G26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5803,10 +5803,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>107</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>106</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>156</v>
@@ -5815,18 +5815,18 @@
         <v>43</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="G2" s="4" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>102</v>
+        <v>34</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>156</v>
@@ -5838,15 +5838,15 @@
         <v>43</v>
       </c>
       <c r="G3" s="4" t="n">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>109</v>
+        <v>35</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>156</v>
@@ -5855,101 +5855,102 @@
         <v>43</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="G4" s="4" t="n">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>156</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G5" s="4" t="n">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>111</v>
+        <v>37</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>156</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="G6" s="4" t="n">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>156</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G7" s="4" t="n">
-        <v>0.3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="A8" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="4" t="n">
-        <v>0.5</v>
+      <c r="D8" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9" t="n">
+        <v>0.9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>36</v>
+        <v>98</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>113</v>
+        <v>38</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>42</v>
@@ -5957,39 +5958,45 @@
       <c r="E9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="4" t="n">
-        <v>0.3</v>
+      <c r="F9" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>114</v>
+        <v>39</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="4" t="n">
-        <v>0.5</v>
+        <v>42</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>37</v>
+        <v>98</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>115</v>
+        <v>38</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>42</v>
@@ -5997,39 +6004,45 @@
       <c r="E11" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="4" t="n">
-        <v>0.6</v>
+      <c r="F11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" s="4" t="n">
-        <v>1</v>
+      <c r="A12" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>38</v>
+        <v>99</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>117</v>
+        <v>36</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>42</v>
@@ -6037,267 +6050,270 @@
       <c r="E13" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="4" t="n">
-        <v>2</v>
+      <c r="F13" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>118</v>
+        <v>37</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="4" t="n">
-        <v>0.4</v>
+        <v>42</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9" t="n">
-        <v>0.9</v>
+      <c r="A15" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="A16" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>159</v>
+      <c r="D16" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>157</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>157</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>38</v>
+        <v>171</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="9" t="s">
+      <c r="A19" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>162</v>
+      <c r="D19" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>36</v>
+        <v>102</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>157</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>163</v>
+        <v>102</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>157</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>165</v>
+        <v>34</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="4" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>170</v>
+      <c r="C24" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9" t="n">
+        <v>0.8</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="C25" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>43</v>
@@ -6305,163 +6321,7 @@
       <c r="E25" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F25" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G30" s="4" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9" t="n">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G32" s="4" t="n">
+      <c r="G25" s="4" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix: added OppositeProcessorType in FactorType
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/v2/15_graph_solver_example.xlsx
+++ b/backend_tests/z_input_files/v2/15_graph_solver_example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="178">
   <si>
     <t xml:space="preserve">Parameter</t>
   </si>
@@ -1032,7 +1032,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -2262,7 +2262,7 @@
   <dimension ref="A1:V40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2870,7 +2870,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="8.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="6.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="6.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="6.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="10.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="13.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="5.96"/>
@@ -2966,9 +2966,6 @@
       <c r="G2" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="L2" s="4" t="n">
         <v>0.1285149</v>
       </c>
@@ -2989,9 +2986,6 @@
       <c r="G3" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="L3" s="4" t="n">
         <v>0.1164551</v>
       </c>
@@ -3012,9 +3006,6 @@
       <c r="G4" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="L4" s="4" t="n">
         <v>0.0810668396092578</v>
       </c>
@@ -3035,9 +3026,6 @@
       <c r="G5" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="L5" s="4" t="n">
         <v>0.0810241451952682</v>
       </c>
@@ -3058,9 +3046,6 @@
       <c r="G6" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="L6" s="4" t="n">
         <v>0.0125177909103313</v>
       </c>
@@ -3081,9 +3066,6 @@
       <c r="G7" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="L7" s="4" t="n">
         <v>0.0125698253799858</v>
       </c>
@@ -3104,9 +3086,6 @@
       <c r="G8" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="L8" s="4" t="n">
         <v>0.290807572629191</v>
       </c>
@@ -3127,9 +3106,6 @@
       <c r="G9" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H9" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="L9" s="4" t="n">
         <v>0.284819139846198</v>
       </c>
@@ -3150,9 +3126,6 @@
       <c r="G10" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H10" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="L10" s="4" t="n">
         <v>510.783090193891</v>
       </c>
@@ -3173,9 +3146,6 @@
       <c r="G11" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H11" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="L11" s="4" t="n">
         <v>510.783090193891</v>
       </c>
@@ -3196,9 +3166,6 @@
       <c r="G12" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H12" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="L12" s="4" t="n">
         <v>344.554124680908</v>
       </c>
@@ -3219,9 +3186,6 @@
       <c r="G13" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H13" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="L13" s="4" t="n">
         <v>344.554124680908</v>
       </c>
@@ -3242,9 +3206,6 @@
       <c r="G14" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H14" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="L14" s="4" t="n">
         <v>54.7726040228444</v>
       </c>
@@ -3265,9 +3226,6 @@
       <c r="G15" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H15" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="L15" s="4" t="n">
         <v>54.7726040228444</v>
       </c>
@@ -3288,9 +3246,6 @@
       <c r="G16" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H16" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="L16" s="4" t="n">
         <v>876.195771627155</v>
       </c>
@@ -3311,9 +3266,6 @@
       <c r="G17" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H17" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="L17" s="4" t="n">
         <v>876.195771627155</v>
       </c>
@@ -3334,9 +3286,6 @@
       <c r="G18" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H18" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="R18" s="4" t="s">
         <v>38</v>
       </c>
@@ -3354,9 +3303,6 @@
       <c r="G19" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H19" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="R19" s="4" t="s">
         <v>38</v>
       </c>
@@ -3374,9 +3320,6 @@
       <c r="G20" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H20" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="L20" s="4" t="n">
         <v>16.2712344327208</v>
       </c>
@@ -3397,9 +3340,6 @@
       <c r="G21" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H21" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="L21" s="4" t="n">
         <v>16.2712344327208</v>
       </c>
@@ -3420,9 +3360,6 @@
       <c r="G22" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H22" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="L22" s="4" t="n">
         <v>0.219509168287431</v>
       </c>
@@ -3443,9 +3380,6 @@
       <c r="G23" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H23" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="L23" s="4" t="n">
         <v>0.219509168287431</v>
       </c>
@@ -3466,9 +3400,6 @@
       <c r="G24" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H24" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="R24" s="4" t="s">
         <v>34</v>
       </c>
@@ -3485,9 +3416,6 @@
       </c>
       <c r="G25" s="4" t="s">
         <v>132</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="R25" s="4" t="s">
         <v>34</v>
@@ -4314,8 +4242,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H38" activeCellId="0" sqref="H38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4423,9 +4351,6 @@
       <c r="G2" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="H2" s="0" t="s">
-        <v>49</v>
-      </c>
       <c r="L2" s="0" t="n">
         <v>14.639493</v>
       </c>
@@ -4447,9 +4372,6 @@
       <c r="G3" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>49</v>
-      </c>
       <c r="L3" s="0" t="n">
         <v>7.7147</v>
       </c>
@@ -4551,9 +4473,6 @@
       <c r="G8" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="H8" s="0" t="s">
-        <v>49</v>
-      </c>
       <c r="L8" s="0" t="n">
         <v>0.423619</v>
       </c>
@@ -4574,9 +4493,6 @@
       <c r="G9" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="H9" s="0" t="s">
-        <v>49</v>
-      </c>
       <c r="L9" s="0" t="n">
         <v>0.198178</v>
       </c>
@@ -4678,9 +4594,6 @@
       <c r="G14" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="H14" s="0" t="s">
-        <v>49</v>
-      </c>
       <c r="L14" s="0" t="n">
         <v>0.483017507961291</v>
       </c>
@@ -4701,9 +4614,6 @@
       <c r="G15" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="H15" s="0" t="s">
-        <v>49</v>
-      </c>
       <c r="L15" s="0" t="n">
         <v>0.318721995608352</v>
       </c>
@@ -4805,9 +4715,6 @@
       <c r="G20" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="H20" s="0" t="s">
-        <v>49</v>
-      </c>
       <c r="L20" s="0" t="n">
         <v>31.1</v>
       </c>
@@ -4828,9 +4735,6 @@
       <c r="G21" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="H21" s="0" t="s">
-        <v>49</v>
-      </c>
       <c r="L21" s="0" t="n">
         <v>21.2</v>
       </c>
@@ -4932,9 +4836,6 @@
       <c r="G26" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="H26" s="0" t="s">
-        <v>49</v>
-      </c>
       <c r="L26" s="0" t="n">
         <v>11.000603</v>
       </c>
@@ -4955,9 +4856,6 @@
       <c r="G27" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="H27" s="0" t="s">
-        <v>49</v>
-      </c>
       <c r="L27" s="0" t="n">
         <v>1.1</v>
       </c>
@@ -5059,9 +4957,6 @@
       <c r="G32" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="H32" s="0" t="s">
-        <v>49</v>
-      </c>
       <c r="L32" s="0" t="n">
         <v>4.388</v>
       </c>
@@ -5082,9 +4977,6 @@
       <c r="G33" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="H33" s="0" t="s">
-        <v>49</v>
-      </c>
       <c r="L33" s="0" t="n">
         <v>4.34</v>
       </c>
@@ -5186,9 +5078,6 @@
       <c r="G38" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="H38" s="0" t="s">
-        <v>49</v>
-      </c>
       <c r="L38" s="0" t="n">
         <v>8.69</v>
       </c>
@@ -5208,9 +5097,6 @@
       </c>
       <c r="G39" s="0" t="s">
         <v>133</v>
-      </c>
-      <c r="H39" s="0" t="s">
-        <v>49</v>
       </c>
       <c r="L39" s="0" t="n">
         <v>2.79</v>
@@ -5763,7 +5649,7 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Dealing with two interfaces with same type but different name
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/v2/15_graph_solver_example.xlsx
+++ b/backend_tests/z_input_files/v2/15_graph_solver_example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="180">
   <si>
     <t xml:space="preserve">Parameter</t>
   </si>
@@ -436,6 +436,12 @@
   </si>
   <si>
     <t xml:space="preserve">Sugarbeet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BlueWaterIn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BlueWaterOut</t>
   </si>
   <si>
     <t xml:space="preserve">OriginProcessors</t>
@@ -754,7 +760,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="C3 A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -856,7 +862,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="1" sqref="C3 C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1032,8 +1038,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="C3 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1604,7 +1610,7 @@
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="C3 B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2262,7 +2268,7 @@
   <dimension ref="A1:V40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="topLeft" activeCell="K1" activeCellId="1" sqref="C3 K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2860,7 +2866,7 @@
   <dimension ref="A1:V65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="1" sqref="C3 G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2872,7 +2878,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="6.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="6.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="10.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="13.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="10.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="5.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="5.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="4" width="5.55"/>
@@ -4242,20 +4248,20 @@
   </sheetPr>
   <dimension ref="A1:AMJ43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="14.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.94"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="5.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="4.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.2"/>
@@ -4264,7 +4270,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="3.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="4.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="0" width="4.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="15.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="5.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="7.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="16.54"/>
@@ -4344,7 +4350,9 @@
       <c r="B2" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="12" t="s">
+        <v>136</v>
+      </c>
       <c r="D2" s="4" t="s">
         <v>107</v>
       </c>
@@ -4365,7 +4373,9 @@
       <c r="B3" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="12"/>
+      <c r="C3" s="12" t="s">
+        <v>137</v>
+      </c>
       <c r="D3" s="4" t="s">
         <v>107</v>
       </c>
@@ -4467,6 +4477,9 @@
       <c r="B8" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="C8" s="12" t="s">
+        <v>136</v>
+      </c>
       <c r="D8" s="4" t="s">
         <v>109</v>
       </c>
@@ -4487,6 +4500,9 @@
       <c r="B9" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="C9" s="12" t="s">
+        <v>137</v>
+      </c>
       <c r="D9" s="4" t="s">
         <v>109</v>
       </c>
@@ -4588,6 +4604,9 @@
       <c r="B14" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="C14" s="12" t="s">
+        <v>136</v>
+      </c>
       <c r="D14" s="4" t="s">
         <v>111</v>
       </c>
@@ -4608,6 +4627,9 @@
       <c r="B15" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="C15" s="12" t="s">
+        <v>137</v>
+      </c>
       <c r="D15" s="4" t="s">
         <v>111</v>
       </c>
@@ -4709,6 +4731,9 @@
       <c r="B20" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="C20" s="12" t="s">
+        <v>136</v>
+      </c>
       <c r="D20" s="4" t="s">
         <v>113</v>
       </c>
@@ -4729,6 +4754,9 @@
       <c r="B21" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="C21" s="12" t="s">
+        <v>137</v>
+      </c>
       <c r="D21" s="4" t="s">
         <v>113</v>
       </c>
@@ -4830,6 +4858,9 @@
       <c r="B26" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="C26" s="12" t="s">
+        <v>136</v>
+      </c>
       <c r="D26" s="4" t="s">
         <v>115</v>
       </c>
@@ -4850,6 +4881,9 @@
       <c r="B27" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="C27" s="12" t="s">
+        <v>137</v>
+      </c>
       <c r="D27" s="4" t="s">
         <v>115</v>
       </c>
@@ -4951,6 +4985,9 @@
       <c r="B32" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="C32" s="12" t="s">
+        <v>136</v>
+      </c>
       <c r="D32" s="4" t="s">
         <v>117</v>
       </c>
@@ -4971,6 +5008,9 @@
       <c r="B33" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="C33" s="12" t="s">
+        <v>137</v>
+      </c>
       <c r="D33" s="4" t="s">
         <v>117</v>
       </c>
@@ -5072,6 +5112,9 @@
       <c r="B38" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="C38" s="12" t="s">
+        <v>136</v>
+      </c>
       <c r="D38" s="4" t="s">
         <v>119</v>
       </c>
@@ -5091,6 +5134,9 @@
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="3" t="s">
         <v>53</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>137</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>119</v>
@@ -5207,7 +5253,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="1" sqref="C3 A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5229,37 +5275,37 @@
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="22.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>6</v>
@@ -5279,7 +5325,7 @@
         <v>33</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5296,7 +5342,7 @@
         <v>34</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5313,7 +5359,7 @@
         <v>35</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5330,7 +5376,7 @@
         <v>36</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5347,7 +5393,7 @@
         <v>37</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5364,7 +5410,7 @@
         <v>38</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5383,7 +5429,7 @@
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -5405,7 +5451,7 @@
         <v>43</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5422,7 +5468,7 @@
         <v>43</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5439,7 +5485,7 @@
         <v>43</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5456,7 +5502,7 @@
         <v>42</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5473,7 +5519,7 @@
         <v>42</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5490,7 +5536,7 @@
         <v>42</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5509,7 +5555,7 @@
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
@@ -5531,10 +5577,10 @@
         <v>42</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5551,10 +5597,10 @@
         <v>43</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5571,7 +5617,7 @@
         <v>42</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5588,7 +5634,7 @@
         <v>43</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5605,7 +5651,7 @@
         <v>42</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="I20" s="12" t="s">
         <v>13</v>
@@ -5625,7 +5671,7 @@
         <v>43</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="I21" s="0" t="s">
         <v>12</v>
@@ -5650,7 +5696,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="C3 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5666,25 +5712,25 @@
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5695,7 +5741,7 @@
         <v>107</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>43</v>
@@ -5715,7 +5761,7 @@
         <v>109</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>43</v>
@@ -5735,7 +5781,7 @@
         <v>111</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>43</v>
@@ -5755,7 +5801,7 @@
         <v>113</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>42</v>
@@ -5775,7 +5821,7 @@
         <v>115</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>42</v>
@@ -5795,7 +5841,7 @@
         <v>117</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>42</v>
@@ -5815,7 +5861,7 @@
         <v>119</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>42</v>
@@ -5836,7 +5882,7 @@
         <v>38</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>42</v>
@@ -5845,10 +5891,10 @@
         <v>42</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5859,7 +5905,7 @@
         <v>39</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>42</v>
@@ -5868,10 +5914,10 @@
         <v>42</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5882,7 +5928,7 @@
         <v>38</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>42</v>
@@ -5894,7 +5940,7 @@
         <v>38</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5905,7 +5951,7 @@
         <v>39</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>42</v>
@@ -5917,7 +5963,7 @@
         <v>39</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5928,7 +5974,7 @@
         <v>36</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>42</v>
@@ -5937,10 +5983,10 @@
         <v>42</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5951,7 +5997,7 @@
         <v>37</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>42</v>
@@ -5960,10 +6006,10 @@
         <v>42</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5974,7 +6020,7 @@
         <v>36</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>42</v>
@@ -5986,7 +6032,7 @@
         <v>36</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5997,7 +6043,7 @@
         <v>37</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>42</v>
@@ -6009,7 +6055,7 @@
         <v>37</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6020,7 +6066,7 @@
         <v>102</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>43</v>
@@ -6029,10 +6075,10 @@
         <v>43</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6043,7 +6089,7 @@
         <v>34</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>43</v>
@@ -6052,10 +6098,10 @@
         <v>43</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6066,7 +6112,7 @@
         <v>35</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>43</v>
@@ -6075,10 +6121,10 @@
         <v>43</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6089,7 +6135,7 @@
         <v>102</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>43</v>
@@ -6101,7 +6147,7 @@
         <v>102</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6112,7 +6158,7 @@
         <v>34</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>43</v>
@@ -6124,7 +6170,7 @@
         <v>34</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6135,7 +6181,7 @@
         <v>35</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>43</v>
@@ -6147,7 +6193,7 @@
         <v>35</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6158,7 +6204,7 @@
         <v>98</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>42</v>
@@ -6178,7 +6224,7 @@
         <v>99</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>42</v>
@@ -6199,7 +6245,7 @@
         <v>100</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Added Orientation checking to command Relationships Updating Biofuel Excel
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/v2/15_graph_solver_example.xlsx
+++ b/backend_tests/z_input_files/v2/15_graph_solver_example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="178">
   <si>
     <t xml:space="preserve">Parameter</t>
   </si>
@@ -454,12 +454,6 @@
   </si>
   <si>
     <t xml:space="preserve">DestinationInterface</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Origin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Destination</t>
   </si>
   <si>
     <t xml:space="preserve">RelationType</t>
@@ -760,7 +754,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="C3 A6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -862,7 +856,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="1" sqref="C3 C13"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1039,7 +1033,7 @@
   <dimension ref="A1:AMJ26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="C3 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1609,8 +1603,8 @@
   </sheetPr>
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="C3 B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2268,7 +2262,7 @@
   <dimension ref="A1:V40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K1" activeCellId="1" sqref="C3 K1"/>
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2866,7 +2860,7 @@
   <dimension ref="A1:V65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="1" sqref="C3 G4"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4248,7 +4242,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -5250,10 +5244,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:AMJ21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="1" sqref="C3 A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5262,15 +5256,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="15.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="19.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="18.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="6.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="10.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="12.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="9.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="23.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="15.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="4" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="4" width="10.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="4" width="15.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="12.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="9.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="23.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="15.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="19.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="11" style="4" width="15.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="22.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5302,14 +5295,10 @@
         <v>146</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="L1" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
@@ -5324,8 +5313,8 @@
       <c r="D2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>149</v>
+      <c r="E2" s="4" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5341,8 +5330,8 @@
       <c r="D3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>149</v>
+      <c r="E3" s="4" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5358,8 +5347,8 @@
       <c r="D4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>149</v>
+      <c r="E4" s="4" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5375,8 +5364,8 @@
       <c r="D5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>149</v>
+      <c r="E5" s="4" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5392,8 +5381,8 @@
       <c r="D6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>149</v>
+      <c r="E6" s="4" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5409,8 +5398,8 @@
       <c r="D7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>149</v>
+      <c r="E7" s="4" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5426,16 +5415,14 @@
       <c r="D8" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="9"/>
+      <c r="E8" s="9" t="s">
+        <v>147</v>
+      </c>
       <c r="F8" s="9"/>
-      <c r="G8" s="9" t="s">
-        <v>149</v>
-      </c>
+      <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
@@ -5450,8 +5437,8 @@
       <c r="D9" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>149</v>
+      <c r="E9" s="4" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5467,8 +5454,8 @@
       <c r="D10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>149</v>
+      <c r="E10" s="4" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5484,8 +5471,8 @@
       <c r="D11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>149</v>
+      <c r="E11" s="4" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5501,8 +5488,8 @@
       <c r="D12" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>149</v>
+      <c r="E12" s="4" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5518,8 +5505,8 @@
       <c r="D13" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>149</v>
+      <c r="E13" s="4" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5535,8 +5522,8 @@
       <c r="D14" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>149</v>
+      <c r="E14" s="4" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5552,16 +5539,14 @@
       <c r="D15" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="9"/>
+      <c r="E15" s="9" t="s">
+        <v>147</v>
+      </c>
       <c r="F15" s="9"/>
-      <c r="G15" s="9" t="s">
-        <v>149</v>
-      </c>
+      <c r="G15" s="9"/>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
@@ -5576,11 +5561,11 @@
       <c r="D16" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>150</v>
+      <c r="E16" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5596,11 +5581,11 @@
       <c r="D17" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="E17" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5616,8 +5601,8 @@
       <c r="D18" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G18" s="4" t="s">
-        <v>149</v>
+      <c r="E18" s="4" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5633,8 +5618,8 @@
       <c r="D19" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G19" s="4" t="s">
-        <v>149</v>
+      <c r="E19" s="4" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5650,10 +5635,10 @@
       <c r="D20" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G20" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="I20" s="12" t="s">
+      <c r="E20" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G20" s="12" t="s">
         <v>13</v>
       </c>
     </row>
@@ -5670,10 +5655,10 @@
       <c r="D21" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G21" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="I21" s="0" t="s">
+      <c r="E21" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G21" s="0" t="s">
         <v>12</v>
       </c>
     </row>
@@ -5696,7 +5681,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="C3 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5712,25 +5697,25 @@
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>156</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5741,7 +5726,7 @@
         <v>107</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>43</v>
@@ -5761,7 +5746,7 @@
         <v>109</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>43</v>
@@ -5781,7 +5766,7 @@
         <v>111</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>43</v>
@@ -5801,7 +5786,7 @@
         <v>113</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>42</v>
@@ -5821,7 +5806,7 @@
         <v>115</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>42</v>
@@ -5841,7 +5826,7 @@
         <v>117</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>42</v>
@@ -5861,7 +5846,7 @@
         <v>119</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>42</v>
@@ -5882,19 +5867,19 @@
         <v>38</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>159</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5905,7 +5890,7 @@
         <v>39</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>42</v>
@@ -5914,10 +5899,10 @@
         <v>42</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5928,7 +5913,7 @@
         <v>38</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>42</v>
@@ -5940,7 +5925,7 @@
         <v>38</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5951,7 +5936,7 @@
         <v>39</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>42</v>
@@ -5963,7 +5948,7 @@
         <v>39</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5974,7 +5959,7 @@
         <v>36</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>42</v>
@@ -5983,10 +5968,10 @@
         <v>42</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5997,7 +5982,7 @@
         <v>37</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>42</v>
@@ -6006,10 +5991,10 @@
         <v>42</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6020,7 +6005,7 @@
         <v>36</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>42</v>
@@ -6032,7 +6017,7 @@
         <v>36</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6043,7 +6028,7 @@
         <v>37</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>42</v>
@@ -6055,7 +6040,7 @@
         <v>37</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6066,7 +6051,7 @@
         <v>102</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>43</v>
@@ -6075,10 +6060,10 @@
         <v>43</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6089,7 +6074,7 @@
         <v>34</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>43</v>
@@ -6098,10 +6083,10 @@
         <v>43</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6112,7 +6097,7 @@
         <v>35</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>43</v>
@@ -6121,10 +6106,10 @@
         <v>43</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6135,7 +6120,7 @@
         <v>102</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>43</v>
@@ -6147,7 +6132,7 @@
         <v>102</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6158,7 +6143,7 @@
         <v>34</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>43</v>
@@ -6170,7 +6155,7 @@
         <v>34</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6181,7 +6166,7 @@
         <v>35</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>43</v>
@@ -6193,7 +6178,7 @@
         <v>35</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6204,7 +6189,7 @@
         <v>98</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>42</v>
@@ -6224,7 +6209,7 @@
         <v>99</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>42</v>
@@ -6245,7 +6230,7 @@
         <v>100</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>43</v>

</xml_diff>